<commit_message>
Ajuste na disposição da logo e leitura de coluta 'target' do arquivo dedos
</commit_message>
<xml_diff>
--- a/super_herois.xlsx
+++ b/super_herois.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\arquivo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmbvrr-my.sharepoint.com/personal/jadir_lima_prefeitura_boavista_br/Documents/SMTI/sorteio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53D45D1-4A49-4D8E-B9BF-4C07CE3ED0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8A398DAC-9A66-4467-B8DC-89D3771A6D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C848B000-B7BB-4385-9A9C-EAAC0D1C7B2B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>nome</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Superman</t>
   </si>
@@ -65,6 +62,42 @@
   </si>
   <si>
     <t>Falcão Noturno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flash </t>
+  </si>
+  <si>
+    <t>Spider Man</t>
+  </si>
+  <si>
+    <t>Hulk</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
+  </si>
+  <si>
+    <t>Deadpool</t>
+  </si>
+  <si>
+    <t>Pantera Negra</t>
+  </si>
+  <si>
+    <t>Adão Negro</t>
+  </si>
+  <si>
+    <t>Demolidor</t>
+  </si>
+  <si>
+    <t>Doutor Strange</t>
+  </si>
+  <si>
+    <t>Viúva negra</t>
+  </si>
+  <si>
+    <t>Green Arrow</t>
+  </si>
+  <si>
+    <t>target</t>
   </si>
 </sst>
 </file>
@@ -595,7 +628,18 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -905,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,80 +962,138 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>